<commit_message>
Changes in excel data provide and jar in pom file.
1) Added DataFormatter class to convert any type of cell to string
value.
2) Update poi jar to 4.0.1.
3) Updated Listener lib to get test case name using result.getName().
4) Added searchPropertyAndPrintAllPricesTest for finding property price
lists out of search results.
</commit_message>
<xml_diff>
--- a/src/test/resources/zoopla_UK_data.xlsx
+++ b/src/test/resources/zoopla_UK_data.xlsx
@@ -69,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +355,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,30 +372,31 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>